<commit_message>
Update BOM total and Executed Test cases
</commit_message>
<xml_diff>
--- a/Documents/BOM.xlsx
+++ b/Documents/BOM.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Hau\Desktop\HW\PSU\Winter16\ECE412 - Capstone\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\OneDrive\HW\Winter16\Capstone\GitHub\QC1.0\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7800" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7800"/>
   </bookViews>
   <sheets>
     <sheet name="BOM Per Unit" sheetId="1" r:id="rId1"/>
     <sheet name="Provided BOM" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="164">
   <si>
     <t>Component</t>
   </si>
@@ -514,6 +514,9 @@
   </si>
   <si>
     <t>DX7s</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -1046,34 +1049,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:P20"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="13.578125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="1.42578125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="23.85546875" style="8" customWidth="1"/>
-    <col min="3" max="3" width="23.85546875" style="8" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" style="2"/>
+    <col min="1" max="1" width="1.41796875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="23.83984375" style="8" customWidth="1"/>
+    <col min="3" max="3" width="23.83984375" style="8" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="13.578125" style="2"/>
     <col min="5" max="5" width="0" style="2" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="27.85546875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="30.140625" style="6" customWidth="1"/>
-    <col min="8" max="8" width="30.140625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="29.5703125" style="2" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="24.85546875" style="2" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="34.42578125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="59.7109375" style="2" customWidth="1"/>
-    <col min="13" max="13" width="37.28515625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="37.28515625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="13.5703125" style="4"/>
-    <col min="16" max="16" width="19.140625" style="5" customWidth="1"/>
-    <col min="17" max="16384" width="13.5703125" style="2"/>
+    <col min="6" max="6" width="27.83984375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="30.15625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="30.15625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="29.578125" style="2" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="24.83984375" style="2" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="34.41796875" style="2" customWidth="1"/>
+    <col min="12" max="12" width="59.68359375" style="2" customWidth="1"/>
+    <col min="13" max="13" width="37.26171875" style="2" customWidth="1"/>
+    <col min="14" max="14" width="37.26171875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="13.578125" style="4"/>
+    <col min="16" max="16" width="19.15625" style="5" customWidth="1"/>
+    <col min="17" max="16384" width="13.578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:16" ht="7.5" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="2" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="9" t="s">
         <v>15</v>
       </c>
@@ -1120,7 +1123,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="7" t="s">
         <v>30</v>
       </c>
@@ -1167,7 +1170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" s="7" t="s">
         <v>30</v>
       </c>
@@ -1214,7 +1217,7 @@
         <v>26.9</v>
       </c>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" s="7" t="s">
         <v>30</v>
       </c>
@@ -1261,7 +1264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" s="7" t="s">
         <v>30</v>
       </c>
@@ -1308,7 +1311,7 @@
         <v>1.93</v>
       </c>
     </row>
-    <row r="7" spans="2:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" s="7" t="s">
         <v>30</v>
       </c>
@@ -1344,7 +1347,7 @@
         <v>82.99</v>
       </c>
     </row>
-    <row r="8" spans="2:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B8" s="7" t="s">
         <v>50</v>
       </c>
@@ -1380,7 +1383,7 @@
         <v>1.35</v>
       </c>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" s="7" t="s">
         <v>30</v>
       </c>
@@ -1416,7 +1419,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="2:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="7" t="s">
         <v>30</v>
       </c>
@@ -1452,7 +1455,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="2:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" s="7" t="s">
         <v>30</v>
       </c>
@@ -1485,7 +1488,7 @@
         <v>74.95</v>
       </c>
     </row>
-    <row r="12" spans="2:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B12" s="7" t="s">
         <v>30</v>
       </c>
@@ -1518,7 +1521,7 @@
         <v>12.71</v>
       </c>
     </row>
-    <row r="13" spans="2:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B13" s="7" t="s">
         <v>50</v>
       </c>
@@ -1554,7 +1557,7 @@
         <v>3.06</v>
       </c>
     </row>
-    <row r="14" spans="2:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B14" s="7" t="s">
         <v>50</v>
       </c>
@@ -1590,7 +1593,7 @@
         <v>0.36749999999999999</v>
       </c>
     </row>
-    <row r="15" spans="2:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" s="7" t="s">
         <v>50</v>
       </c>
@@ -1626,7 +1629,7 @@
         <v>0.20250000000000001</v>
       </c>
     </row>
-    <row r="16" spans="2:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B16" s="7" t="s">
         <v>50</v>
       </c>
@@ -1662,7 +1665,7 @@
         <v>0.18473000000000001</v>
       </c>
     </row>
-    <row r="17" spans="2:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B17" s="7" t="s">
         <v>50</v>
       </c>
@@ -1698,7 +1701,7 @@
         <v>6.8849999999999995E-2</v>
       </c>
     </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B18" s="7" t="s">
         <v>50</v>
       </c>
@@ -1734,17 +1737,28 @@
         <v>1.33</v>
       </c>
     </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
       <c r="L19" s="3"/>
       <c r="M19" s="3"/>
     </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
+      <c r="N20" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="O20" s="4">
+        <f>SUM(O3:O18)</f>
+        <v>267.43</v>
+      </c>
+      <c r="P20" s="4">
+        <f>SUM(P3:P18)</f>
+        <v>263.04357999999996</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1789,19 +1803,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="45" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5703125" customWidth="1"/>
+    <col min="2" max="2" width="24.41796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.578125" customWidth="1"/>
     <col min="4" max="4" width="67" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>108</v>
       </c>
@@ -1815,7 +1829,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>112</v>
       </c>
@@ -1826,7 +1840,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>114</v>
       </c>
@@ -1840,7 +1854,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>116</v>
       </c>
@@ -1851,7 +1865,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>118</v>
       </c>
@@ -1865,7 +1879,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>119</v>
       </c>
@@ -1879,7 +1893,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>122</v>
       </c>
@@ -1893,7 +1907,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>125</v>
       </c>
@@ -1901,7 +1915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>126</v>
       </c>
@@ -1912,7 +1926,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>128</v>
       </c>
@@ -1923,7 +1937,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>130</v>
       </c>
@@ -1934,7 +1948,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>131</v>
       </c>
@@ -1945,7 +1959,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>133</v>
       </c>
@@ -1959,7 +1973,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>136</v>
       </c>
@@ -1973,7 +1987,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>139</v>
       </c>
@@ -1987,7 +2001,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>142</v>
       </c>
@@ -2001,7 +2015,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>145</v>
       </c>
@@ -2015,7 +2029,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>63</v>
       </c>
@@ -2026,7 +2040,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>148</v>
       </c>
@@ -2037,7 +2051,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>56</v>
       </c>
@@ -2048,7 +2062,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>68</v>
       </c>
@@ -2056,7 +2070,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>151</v>
       </c>
@@ -2070,7 +2084,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>153</v>
       </c>
@@ -2081,7 +2095,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>154</v>
       </c>
@@ -2092,7 +2106,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>155</v>
       </c>
@@ -2103,7 +2117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>156</v>
       </c>
@@ -2114,7 +2128,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>157</v>
       </c>
@@ -2128,7 +2142,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>159</v>
       </c>
@@ -2139,7 +2153,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>161</v>
       </c>

</xml_diff>